<commit_message>
extra comments & small changes
</commit_message>
<xml_diff>
--- a/Classification Results.xlsx
+++ b/Classification Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrian\Desktop\Expected Goals Project Part 2 - Electric Boogaloo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrian\Desktop\FootballAnalyticsML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A6C6CC-0041-4450-9462-FB74EB5DCEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0695AE-719A-4D88-8E6C-DB2931A364F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{96F4CFBF-A1EA-4E15-91D5-D7E45775CD89}"/>
+    <workbookView xWindow="348" yWindow="3756" windowWidth="17280" windowHeight="10044" xr2:uid="{96F4CFBF-A1EA-4E15-91D5-D7E45775CD89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,9 +570,7 @@
       <c r="B7" s="2">
         <v>0.88</v>
       </c>
-      <c r="C7" s="2">
-        <v>0.73</v>
-      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="2">
         <v>0.33</v>
       </c>

</xml_diff>